<commit_message>
program creates a xlsx file of hyperlinks to web articles
</commit_message>
<xml_diff>
--- a/news.xlsx
+++ b/news.xlsx
@@ -1,43 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Заглушават GPS сигналите покрай българското крайбрежие – източникът за сега е неизвестен</t>
+  </si>
+  <si>
+    <t>Проучване: 6G технологията ще се предава чрез … хората</t>
+  </si>
+  <si>
+    <t>System76 Pangolin: идеалният лаптоп за програмиста с Ryzen 7 6800U, 144 Hz дисплей и Ubuntu 22.04</t>
+  </si>
+  <si>
+    <t>Intel чупи бариерата от 6GHz с процесора Core i9-13900KS с цена 699 долара</t>
+  </si>
+  <si>
+    <t>Lenovo ThinkPad Z13: Еволюция в действие</t>
+  </si>
+  <si>
+    <t>НАСА работи върху хибридната мисия до Титан и още над дузина проекти в космоса</t>
+  </si>
+  <si>
+    <t>Историческото първо изстрелване на ракета от британска територия претърпя провал</t>
+  </si>
+  <si>
+    <t>Razer допълва линията си лаптопи с високотехнологичните Blade 16 и Blade 18</t>
+  </si>
+  <si>
+    <t>Срокът за кандидатстване за космическия лагер Space Camp Turkey се удължава</t>
+  </si>
+  <si>
+    <t>Русия ще остави Союз в орбита! Ще издигне нов кораб, който да прибере руските астронавти на Земята</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,94 +82,24 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,137 +387,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Ето как ChatGPT вместо мен реши теста по програмиране в интервюто за започване на работа</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>IMG DXT: нов мобилен графичен процесор с поддръжка на трасирането на лъчите</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Заглушават GPS сигналите покрай българското крайбрежие – източникът за сега е неизвестен</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Проучване: 6G технологията ще се предава чрез … хората</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Intel чупи бариерата от 6GHz с процесора Core i9-13900KS с цена 699 долара</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Lenovo ThinkPad Z13: Еволюция в действие</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>НАСА работи върху хибридната мисия до Титан и още над дузина проекти в космоса</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Историческото първо изстрелване на ракета от британска територия претърпя провал</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Razer допълва линията си лаптопи с високотехнологичните Blade 16 и Blade 18</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Срокът за кандидатстване за космическия лагер Space Camp Turkey се удължава</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Русия ще остави Союз в орбита! Ще издигне нов кораб, който да прибере руските астронавти на Земята</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://www.kaldata.com/it-%d0%bd%d0%be%d0%b2%d0%b8%d0%bd%d0%b8/%d0%b5%d1%82%d0%be-%d0%ba%d0%b0%d0%ba-chatgpt-%d0%b2%d0%bc%d0%b5%d1%81%d1%82%d0%be-%d0%bc%d0%b5%d0%bd-%d1%80%d0%b5%d1%88%d0%b8-%d1%82%d0%b5%d1%81%d1%82%d0%b0-%d0%bf%d0%be-%d0%bf%d1%80%d0%be%d0%b3-404070.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://www.kaldata.com/%d1%82%d0%b5%d0%bb%d0%b5%d1%84%d0%be%d0%bd%d0%b8/img-dxt-%d0%bd%d0%be%d0%b2-%d0%bc%d0%be%d0%b1%d0%b8%d0%bb%d0%b5%d0%bd-%d0%b3%d1%80%d0%b0%d1%84%d0%b8%d1%87%d0%b5%d0%bd-%d0%bf%d1%80%d0%be%d1%86%d0%b5%d1%81%d0%be%d1%80-%d1%81-%d0%bf%d0%be%d0%b4%d0%b4-404079.html</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://www.kaldata.com/it-%d0%bd%d0%be%d0%b2%d0%b8%d0%bd%d0%b8/%d0%b7%d0%b0%d0%b3%d0%bb%d1%83%d1%88%d0%b0%d0%b2%d0%b0%d1%82-gps-%d1%81%d0%b8%d0%b3%d0%bd%d0%b0%d0%bb%d0%b8%d1%82%d0%b5-%d0%bf%d0%be%d0%ba%d1%80%d0%b0%d0%b9-%d0%b1%d1%8a%d0%bb%d0%b3%d0%b0%d1%80%d1%81-403838.html</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>https://www.kaldata.com/it-%d0%bd%d0%be%d0%b2%d0%b8%d0%bd%d0%b8/%d0%bf%d1%80%d0%be%d1%83%d1%87%d0%b2%d0%b0%d0%bd%d0%b5-6g-%d1%82%d0%b5%d1%85%d0%bd%d0%be%d0%bb%d0%be%d0%b3%d0%b8%d1%8f%d1%82%d0%b0-%d1%89%d0%b5-%d1%81%d0%b5-%d0%bf%d1%80%d0%b5%d0%b4%d0%b0%d0%b2%d0%b0-403767.html</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>https://www.kaldata.com/%d1%85%d0%b0%d1%80%d0%b4%d1%83%d0%b5%d1%80/intel-%d1%87%d1%83%d0%bf%d0%b8-%d0%b1%d0%b0%d1%80%d0%b8%d0%b5%d1%80%d0%b0%d1%82%d0%b0-%d0%be%d1%82-6ghz-%d1%81-%d0%bf%d1%80%d0%be%d1%86%d0%b5%d1%81%d0%be%d1%80%d0%b0-core-i9-13900ks-%d1%81-%d1%86-404161.html</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>https://www.kaldata.com/%d1%80%d0%b5%d0%b2%d1%8e%d1%82%d0%b0/lenovo-thinkpad-z13-%d0%b5%d0%b2%d0%be%d0%bb%d1%8e%d1%86%d0%b8%d1%8f-%d0%b2-%d0%b4%d0%b5%d0%b9%d1%81%d1%82%d0%b2%d0%b8%d0%b5-399936.html</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>https://www.kaldata.com/it-%d0%bd%d0%be%d0%b2%d0%b8%d0%bd%d0%b8/%d0%ba%d0%be%d1%81%d0%bc%d0%be%d1%81/%d0%bd%d0%b0%d1%81%d0%b0-%d1%80%d0%b0%d0%b1%d0%be%d1%82%d0%b8-%d0%b2%d1%8a%d1%80%d1%85%d1%83-%d1%85%d0%b8%d0%b1%d1%80%d0%b8%d0%b4%d0%bd%d0%b0%d1%82%d0%b0-%d0%bc%d0%b8%d1%81%d0%b8%d1%8f-%d0%b4%d0%be-404112.html</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>https://www.kaldata.com/it-%d0%bd%d0%be%d0%b2%d0%b8%d0%bd%d0%b8/%d0%b8%d1%81%d1%82%d0%be%d1%80%d0%b8%d1%87%d0%b5%d1%81%d0%ba%d0%be%d1%82%d0%be-%d0%bf%d1%8a%d1%80%d0%b2%d0%be-%d0%b8%d0%b7%d1%81%d1%82%d1%80%d0%b5%d0%bb%d0%b2%d0%b0%d0%bd%d0%b5-%d0%bd%d0%b0-%d1%80-403804.html</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>https://www.kaldata.com/%d1%85%d0%b0%d1%80%d0%b4%d1%83%d0%b5%d1%80/razer-%d0%b4%d0%be%d0%bf%d1%8a%d0%bb%d0%b2%d0%b0-%d0%bb%d0%b8%d0%bd%d0%b8%d1%8f%d1%82%d0%b0-%d1%81%d0%b8-%d0%bb%d0%b0%d0%bf%d1%82%d0%be%d0%bf%d0%b8-%d1%81-%d0%b2%d0%b8%d1%81%d0%be%d0%ba%d0%be%d1%82-403336.html</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>https://www.kaldata.com/it-%d0%bd%d0%be%d0%b2%d0%b8%d0%bd%d0%b8/%d0%ba%d0%be%d1%81%d0%bc%d0%be%d1%81/%d1%81%d1%80%d0%be%d0%ba%d1%8a%d1%82-%d0%b7%d0%b0-%d0%ba%d0%b0%d0%bd%d0%b4%d0%b8%d0%b4%d0%b0%d1%82%d1%81%d1%82%d0%b2%d0%b0%d0%bd%d0%b5-%d0%b7%d0%b0-%d0%ba%d0%be%d1%81%d0%bc%d0%b8%d1%87%d0%b5%d1%81-404162.html</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>https://www.kaldata.com/it-%d0%bd%d0%be%d0%b2%d0%b8%d0%bd%d0%b8/%d1%80%d1%83%d1%81%d0%b8%d1%8f-%d1%89%d0%b5-%d0%be%d1%81%d1%82%d0%b0%d0%b2%d0%b8-%d1%81%d0%be%d1%8e%d0%b7-%d0%b2-%d0%be%d1%80%d0%b1%d0%b8%d1%82%d0%b0-%d1%89%d0%b5-%d0%b8%d0%b7%d0%b4%d0%b8%d0%b3%d0%bd-404052.html</t>
-        </is>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" tooltip="open this article"/>
+    <hyperlink ref="A2" r:id="rId2" tooltip="open this article"/>
+    <hyperlink ref="A3" r:id="rId3" tooltip="open this article"/>
+    <hyperlink ref="A4" r:id="rId4" tooltip="open this article"/>
+    <hyperlink ref="A5" r:id="rId5" tooltip="open this article"/>
+    <hyperlink ref="A6" r:id="rId6" tooltip="open this article"/>
+    <hyperlink ref="A7" r:id="rId7" tooltip="open this article"/>
+    <hyperlink ref="A8" r:id="rId8" tooltip="open this article"/>
+    <hyperlink ref="A9" r:id="rId9" tooltip="open this article"/>
+    <hyperlink ref="A10" r:id="rId10" tooltip="open this article"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working program, sends email -includes all homepage articles from kaldata. TODO: make unit tests; format the code; add comments; etc
</commit_message>
<xml_diff>
--- a/news.xlsx
+++ b/news.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>HWO е новият космически телескоп за търсене на извънземен живот</t>
+  </si>
+  <si>
+    <t>Nvidia Broadcast използва ИИ за автоматично регулиране на погледа</t>
+  </si>
+  <si>
+    <t>Нефтопреработвателната компания Exxonmobil е прогнозирала точно изменението на климата, докато публично е отхвърляла това</t>
+  </si>
   <si>
     <t>Заглушават GPS сигналите покрай българското крайбрежие – източникът за сега е неизвестен</t>
   </si>
@@ -22,6 +31,9 @@
     <t>Проучване: 6G технологията ще се предава чрез … хората</t>
   </si>
   <si>
+    <t>Ето как ChatGPT вместо мен реши теста по програмиране в интервюто за започване на работа</t>
+  </si>
+  <si>
     <t>System76 Pangolin: идеалният лаптоп за програмиста с Ryzen 7 6800U, 144 Hz дисплей и Ubuntu 22.04</t>
   </si>
   <si>
@@ -37,13 +49,7 @@
     <t>Историческото първо изстрелване на ракета от британска територия претърпя провал</t>
   </si>
   <si>
-    <t>Razer допълва линията си лаптопи с високотехнологичните Blade 16 и Blade 18</t>
-  </si>
-  <si>
     <t>Срокът за кандидатстване за космическия лагер Space Camp Turkey се удължава</t>
-  </si>
-  <si>
-    <t>Русия ще остави Союз в орбита! Ще издигне нов кораб, който да прибере руските астронавти на Земята</t>
   </si>
 </sst>
 </file>
@@ -388,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -442,6 +448,16 @@
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -456,6 +472,8 @@
     <hyperlink ref="A8" r:id="rId8" tooltip="open this article"/>
     <hyperlink ref="A9" r:id="rId9" tooltip="open this article"/>
     <hyperlink ref="A10" r:id="rId10" tooltip="open this article"/>
+    <hyperlink ref="A11" r:id="rId11" tooltip="open this article"/>
+    <hyperlink ref="A12" r:id="rId12" tooltip="open this article"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
stable version 1.0 - featured websites: Kaldata.com; - email server: outlook
</commit_message>
<xml_diff>
--- a/news.xlsx
+++ b/news.xlsx
@@ -14,42 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Екипажът на Союз МС-22 ще остане още няколко месеца на МКС</t>
+  </si>
+  <si>
+    <t>„Първата извънземна сонда, достигнала Земята, ще бъде твърде сложна, за да я разберем“</t>
+  </si>
+  <si>
+    <t>Заглушават GPS сигналите покрай българското крайбрежие – източникът за сега е неизвестен</t>
+  </si>
+  <si>
+    <t>Lenovo ThinkPad Z13: Еволюция в действие</t>
+  </si>
+  <si>
+    <t>НАСА работи върху хибридната мисия до Титан и още над дузина проекти в космоса</t>
+  </si>
+  <si>
+    <t>Историческото първо изстрелване на ракета от британска територия претърпя провал</t>
+  </si>
   <si>
     <t>HWO е новият космически телескоп за търсене на извънземен живот</t>
-  </si>
-  <si>
-    <t>Nvidia Broadcast използва ИИ за автоматично регулиране на погледа</t>
-  </si>
-  <si>
-    <t>Нефтопреработвателната компания Exxonmobil е прогнозирала точно изменението на климата, докато публично е отхвърляла това</t>
-  </si>
-  <si>
-    <t>Заглушават GPS сигналите покрай българското крайбрежие – източникът за сега е неизвестен</t>
-  </si>
-  <si>
-    <t>Проучване: 6G технологията ще се предава чрез … хората</t>
-  </si>
-  <si>
-    <t>Ето как ChatGPT вместо мен реши теста по програмиране в интервюто за започване на работа</t>
-  </si>
-  <si>
-    <t>System76 Pangolin: идеалният лаптоп за програмиста с Ryzen 7 6800U, 144 Hz дисплей и Ubuntu 22.04</t>
-  </si>
-  <si>
-    <t>Intel чупи бариерата от 6GHz с процесора Core i9-13900KS с цена 699 долара</t>
-  </si>
-  <si>
-    <t>Lenovo ThinkPad Z13: Еволюция в действие</t>
-  </si>
-  <si>
-    <t>НАСА работи върху хибридната мисия до Титан и още над дузина проекти в космоса</t>
-  </si>
-  <si>
-    <t>Историческото първо изстрелване на ракета от британска територия претърпя провал</t>
-  </si>
-  <si>
-    <t>Срокът за кандидатстване за космическия лагер Space Camp Turkey се удължава</t>
   </si>
 </sst>
 </file>
@@ -394,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -433,31 +418,6 @@
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -469,11 +429,6 @@
     <hyperlink ref="A5" r:id="rId5" tooltip="open this article"/>
     <hyperlink ref="A6" r:id="rId6" tooltip="open this article"/>
     <hyperlink ref="A7" r:id="rId7" tooltip="open this article"/>
-    <hyperlink ref="A8" r:id="rId8" tooltip="open this article"/>
-    <hyperlink ref="A9" r:id="rId9" tooltip="open this article"/>
-    <hyperlink ref="A10" r:id="rId10" tooltip="open this article"/>
-    <hyperlink ref="A11" r:id="rId11" tooltip="open this article"/>
-    <hyperlink ref="A12" r:id="rId12" tooltip="open this article"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>